<commit_message>
ajout de l'image par défaut
</commit_message>
<xml_diff>
--- a/Enonce/Backlog.xlsx
+++ b/Enonce/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\OneDrive\GitHub\TP-AppWeb\Enonce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etien\GitHub\TP-AppWeb\Enonce\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="Catalogue-sem-1" sheetId="1" r:id="rId1"/>
     <sheet name="Catalogue-sem-2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <r>
       <t xml:space="preserve">Catalogue produit </t>
@@ -856,6 +856,13 @@
 • Si succès redirection sur la page d'accueil
   et déconnexion dans la navbar deviens 
   login.</t>
+  </si>
+  <si>
+    <t>DÉBUTER
+75%</t>
+  </si>
+  <si>
+    <t>Étienne</t>
   </si>
 </sst>
 </file>
@@ -992,7 +999,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1023,9 +1030,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1121,10 +1125,28 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1412,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
@@ -1422,9 +1444,9 @@
     <col min="2" max="2" width="5.796875" customWidth="1"/>
     <col min="3" max="3" width="6.8984375" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="35.59765625" customWidth="1"/>
+    <col min="5" max="5" width="38.09765625" customWidth="1"/>
     <col min="6" max="6" width="17.3984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.296875" customWidth="1"/>
+    <col min="7" max="7" width="14.296875" style="7" customWidth="1"/>
     <col min="8" max="8" width="31.69921875" customWidth="1"/>
     <col min="9" max="1024" width="8.5" customWidth="1"/>
     <col min="1025" max="1025" width="11.19921875" customWidth="1"/>
@@ -1495,31 +1517,31 @@
       <c r="E12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="49"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:8" ht="110.4">
+      <c r="C13" s="14">
+        <v>2</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-    </row>
-    <row r="13" spans="2:8" ht="110.4">
-      <c r="C13" s="15">
-        <v>2</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16" t="s">
+      <c r="G13" s="52"/>
+      <c r="H13" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="18" customFormat="1" ht="82.8">
+    <row r="14" spans="2:8" s="17" customFormat="1" ht="82.8">
       <c r="C14" s="10">
         <v>3</v>
       </c>
@@ -1529,351 +1551,371 @@
       <c r="E14" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" s="17" customFormat="1" ht="124.2">
+      <c r="C15" s="16">
+        <v>4</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="44"/>
+    </row>
+    <row r="16" spans="2:8" s="17" customFormat="1" ht="82.8">
+      <c r="C16" s="45">
+        <v>5</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="48"/>
+    </row>
+    <row r="17" spans="3:8" s="17" customFormat="1" ht="55.2">
+      <c r="C17" s="16">
+        <v>6</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="18"/>
+    </row>
+    <row r="18" spans="3:8" s="17" customFormat="1" ht="69">
+      <c r="C18" s="45">
+        <v>7</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" s="18" customFormat="1" ht="138">
-      <c r="C15" s="17">
-        <v>4</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="17" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="21"/>
+    </row>
+    <row r="19" spans="3:8" s="23" customFormat="1" ht="55.2">
+      <c r="C19" s="16">
+        <v>8</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="45"/>
-    </row>
-    <row r="16" spans="2:8" s="18" customFormat="1" ht="96.6">
-      <c r="C16" s="46">
-        <v>5</v>
-      </c>
-      <c r="D16" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="G19" s="51"/>
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="3:8" s="17" customFormat="1" ht="69">
+      <c r="C20" s="45">
+        <v>9</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="49"/>
-      <c r="H16" s="50"/>
-    </row>
-    <row r="17" spans="3:8" s="18" customFormat="1" ht="55.2">
-      <c r="C17" s="17">
-        <v>6</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="20" t="s">
+      <c r="G20" s="54"/>
+      <c r="H20" s="21"/>
+    </row>
+    <row r="21" spans="3:8" s="23" customFormat="1" ht="69">
+      <c r="C21" s="16">
+        <v>10</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="51"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="3:8" s="17" customFormat="1" ht="41.4">
+      <c r="C22" s="45">
+        <v>11</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H17" s="19"/>
-    </row>
-    <row r="18" spans="3:8" s="18" customFormat="1" ht="69">
-      <c r="C18" s="46">
-        <v>7</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="21" t="s">
+      <c r="G22" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="3:8" s="23" customFormat="1" ht="69">
+      <c r="C23" s="16">
+        <v>12</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" spans="3:8" s="17" customFormat="1" ht="69">
+      <c r="C24" s="45">
+        <v>13</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="21"/>
+    </row>
+    <row r="25" spans="3:8" s="23" customFormat="1" ht="55.2">
+      <c r="C25" s="16">
+        <v>14</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="18"/>
+    </row>
+    <row r="26" spans="3:8" s="17" customFormat="1" ht="69">
+      <c r="C26" s="45">
+        <v>15</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="21"/>
+    </row>
+    <row r="27" spans="3:8" s="23" customFormat="1" ht="82.8">
+      <c r="C27" s="16">
+        <v>16</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-    </row>
-    <row r="19" spans="3:8" s="24" customFormat="1" ht="55.2">
-      <c r="C19" s="17">
-        <v>8</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="G27" s="51"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="3:8" ht="82.8">
+      <c r="C28" s="45">
+        <v>17</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="3:8" s="18" customFormat="1" ht="69">
-      <c r="C20" s="46">
-        <v>9</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="21" t="s">
+      <c r="G28" s="54"/>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="3:8" s="28" customFormat="1" ht="55.2">
+      <c r="C29" s="16">
+        <v>18</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-    </row>
-    <row r="21" spans="3:8" s="24" customFormat="1" ht="69">
-      <c r="C21" s="17">
-        <v>10</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-    </row>
-    <row r="22" spans="3:8" s="18" customFormat="1" ht="41.4">
-      <c r="C22" s="46">
-        <v>11</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-    </row>
-    <row r="23" spans="3:8" s="24" customFormat="1" ht="69">
-      <c r="C23" s="17">
-        <v>12</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-    </row>
-    <row r="24" spans="3:8" s="18" customFormat="1" ht="82.8">
-      <c r="C24" s="46">
-        <v>13</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-    </row>
-    <row r="25" spans="3:8" s="24" customFormat="1" ht="55.2">
-      <c r="C25" s="17">
-        <v>14</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="3:8" s="18" customFormat="1" ht="69">
-      <c r="C26" s="46">
-        <v>15</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="3:8" s="24" customFormat="1" ht="82.8">
-      <c r="C27" s="17">
-        <v>16</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E27" s="19" t="s">
+      <c r="G29" s="51"/>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="3:8" ht="41.4">
+      <c r="C30" s="45">
+        <v>19</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-    </row>
-    <row r="28" spans="3:8" ht="82.8">
-      <c r="C28" s="46">
-        <v>17</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-    </row>
-    <row r="29" spans="3:8" s="29" customFormat="1" ht="55.2">
-      <c r="C29" s="17">
-        <v>18</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F29" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-    </row>
-    <row r="30" spans="3:8" ht="41.4">
-      <c r="C30" s="46">
-        <v>19</v>
-      </c>
-      <c r="D30" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-    </row>
-    <row r="31" spans="3:8" s="29" customFormat="1" ht="55.2">
-      <c r="C31" s="17">
+      <c r="F30" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" s="21"/>
+    </row>
+    <row r="31" spans="3:8" s="28" customFormat="1" ht="55.2">
+      <c r="C31" s="16">
         <v>20</v>
       </c>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
+      <c r="F31" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31" s="18"/>
     </row>
     <row r="32" spans="3:8">
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="35" spans="2:8">
       <c r="C35" s="1"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="30"/>
     </row>
     <row r="36" spans="2:8">
-      <c r="D36" s="33" t="s">
+      <c r="D36" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="2:8">
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="35"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="2:8">
-      <c r="D38" s="27" t="s">
+      <c r="D38" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E38" s="24"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="2:8">
       <c r="D39" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="2:8">
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E40" s="36"/>
+      <c r="E40" s="35"/>
     </row>
     <row r="41" spans="2:8">
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="36"/>
+      <c r="E41" s="35"/>
     </row>
     <row r="42" spans="2:8">
-      <c r="E42" s="29"/>
+      <c r="E42" s="28"/>
     </row>
     <row r="43" spans="2:8">
-      <c r="D43" s="38" t="s">
+      <c r="D43" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="28"/>
     </row>
     <row r="44" spans="2:8">
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="38" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1950,102 +1992,102 @@
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="15">
       <c r="B11"/>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="40" t="s">
+      <c r="G11" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="40" t="s">
+      <c r="H11" s="39" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="69">
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42" t="s">
+      <c r="E12" s="41"/>
+      <c r="F12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
     </row>
     <row r="13" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>2</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="43" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
     </row>
     <row r="14" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>3</v>
       </c>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
     </row>
     <row r="15" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C15" s="15">
+      <c r="C15" s="14">
         <v>4</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44" t="s">
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
     </row>
     <row r="16" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C16" s="15">
+      <c r="C16" s="14">
         <v>5</v>
       </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="17" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C17" s="15">
+      <c r="C17" s="14">
         <v>6</v>
       </c>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
     </row>
     <row r="18" spans="2:8" ht="46.2" customHeight="1">
-      <c r="C18" s="15"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
     </row>
     <row r="21" spans="2:8">
       <c r="B21" s="5" t="s">

</xml_diff>